<commit_message>
Fixed Excel header mapping and data population - Added fallback logic for missing data - Applied headers to all 3 Excel pages - Fixed year format (25 instead of 2025) - Resolved syntax errors in server.js
</commit_message>
<xml_diff>
--- a/backend/templates/Inline_inspection_form.xlsx
+++ b/backend/templates/Inline_inspection_form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gchar\OneDrive\Desktop\Misc\SwansonIndiaPortal\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gchar\OneDrive\Desktop\Misc\SwansonIndiaPortal\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697214E4-AE19-40BA-B2A9-19AE462D346E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347DE6D4-0361-4134-B4E6-608348858260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="588" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -718,6 +718,33 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -733,38 +760,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -774,57 +777,6 @@
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -865,25 +817,73 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1202,8 +1202,8 @@
   </sheetPr>
   <dimension ref="A1:AM89"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1221,10 +1221,10 @@
         <v>0</v>
       </c>
       <c r="AD1" s="3"/>
-      <c r="AE1" s="87" t="s">
+      <c r="AE1" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="AF1" s="87"/>
+      <c r="AF1" s="38"/>
       <c r="AI1" s="2"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
@@ -1235,260 +1235,260 @@
       <c r="A2" s="1"/>
       <c r="AC2" s="4"/>
       <c r="AD2" s="4"/>
-      <c r="AE2" s="86" t="s">
+      <c r="AE2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="AF2" s="86"/>
+      <c r="AF2" s="37"/>
     </row>
     <row r="3" spans="1:39" s="30" customFormat="1" ht="26.25">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="89"/>
-      <c r="T3" s="89"/>
-      <c r="U3" s="89"/>
-      <c r="V3" s="89"/>
-      <c r="W3" s="89"/>
-      <c r="X3" s="89"/>
-      <c r="Y3" s="89"/>
-      <c r="Z3" s="89"/>
-      <c r="AA3" s="89"/>
-      <c r="AB3" s="89"/>
-      <c r="AC3" s="89"/>
-      <c r="AD3" s="89"/>
-      <c r="AE3" s="89"/>
-      <c r="AF3" s="89"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="41"/>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="41"/>
+      <c r="AD3" s="41"/>
+      <c r="AE3" s="41"/>
+      <c r="AF3" s="41"/>
     </row>
     <row r="4" spans="1:39" s="29" customFormat="1" ht="19.5">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="90"/>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="90"/>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-      <c r="AB4" s="90"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="90"/>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="90"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="42"/>
+      <c r="X4" s="42"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="42"/>
+      <c r="AA4" s="42"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="42"/>
+      <c r="AD4" s="42"/>
+      <c r="AE4" s="42"/>
+      <c r="AF4" s="42"/>
     </row>
     <row r="5" spans="1:39" s="6" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="AC5" s="91"/>
-      <c r="AD5" s="91"/>
-      <c r="AE5" s="92"/>
-      <c r="AF5" s="92"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="AC5" s="44"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="45"/>
+      <c r="AF5" s="45"/>
     </row>
     <row r="6" spans="1:39" s="6" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="J6" s="47" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="J6" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="47"/>
+      <c r="K6" s="51"/>
       <c r="L6" s="27"/>
-      <c r="N6" s="42" t="s">
+      <c r="N6" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="43"/>
-      <c r="P6" s="42" t="s">
+      <c r="O6" s="91"/>
+      <c r="P6" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="42" t="s">
+      <c r="Q6" s="91"/>
+      <c r="R6" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="43"/>
-      <c r="T6" s="42" t="s">
+      <c r="S6" s="91"/>
+      <c r="T6" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="U6" s="43"/>
-      <c r="V6" s="42" t="s">
+      <c r="U6" s="91"/>
+      <c r="V6" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="W6" s="43"/>
-      <c r="AB6" s="45" t="s">
+      <c r="W6" s="91"/>
+      <c r="AB6" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="AC6" s="45"/>
-      <c r="AD6" s="88"/>
-      <c r="AE6" s="44"/>
-      <c r="AF6" s="41"/>
+      <c r="AC6" s="39"/>
+      <c r="AD6" s="40"/>
+      <c r="AE6" s="92"/>
+      <c r="AF6" s="50"/>
     </row>
     <row r="7" spans="1:39" s="6" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="J7" s="47" t="s">
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="J7" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="47"/>
+      <c r="K7" s="51"/>
       <c r="L7" s="27"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="38"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="38"/>
-      <c r="AB7" s="45" t="s">
+      <c r="N7" s="46"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="47"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="47"/>
+      <c r="AB7" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="AC7" s="45"/>
-      <c r="AD7" s="88"/>
-      <c r="AE7" s="41"/>
-      <c r="AF7" s="41"/>
+      <c r="AC7" s="39"/>
+      <c r="AD7" s="40"/>
+      <c r="AE7" s="50"/>
+      <c r="AF7" s="50"/>
     </row>
     <row r="8" spans="1:39" s="6" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="J8" s="47" t="s">
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="J8" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="47"/>
+      <c r="K8" s="51"/>
       <c r="L8" s="27"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="40"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="40"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="40"/>
-      <c r="AB8" s="45" t="s">
+      <c r="N8" s="48"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="49"/>
+      <c r="AB8" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="AC8" s="45"/>
-      <c r="AD8" s="88"/>
-      <c r="AE8" s="41"/>
-      <c r="AF8" s="41"/>
+      <c r="AC8" s="39"/>
+      <c r="AD8" s="40"/>
+      <c r="AE8" s="50"/>
+      <c r="AF8" s="50"/>
     </row>
     <row r="9" spans="1:39" s="6" customFormat="1" ht="6" customHeight="1">
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
     </row>
     <row r="10" spans="1:39" s="7" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="51" t="s">
+      <c r="B10" s="75"/>
+      <c r="C10" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
       <c r="F10" s="31"/>
-      <c r="G10" s="51" t="s">
+      <c r="G10" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="52"/>
+      <c r="H10" s="89"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="51" t="s">
+      <c r="J10" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="K10" s="52"/>
+      <c r="K10" s="89"/>
       <c r="L10" s="32"/>
-      <c r="M10" s="49" t="s">
+      <c r="M10" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="65"/>
-      <c r="O10" s="65"/>
-      <c r="P10" s="65"/>
-      <c r="Q10" s="65"/>
-      <c r="R10" s="65"/>
-      <c r="S10" s="65"/>
-      <c r="T10" s="65"/>
-      <c r="U10" s="65"/>
-      <c r="V10" s="65"/>
-      <c r="W10" s="65"/>
-      <c r="X10" s="65"/>
-      <c r="Y10" s="65"/>
-      <c r="Z10" s="65"/>
-      <c r="AA10" s="65"/>
-      <c r="AB10" s="50"/>
-      <c r="AC10" s="66" t="s">
+      <c r="N10" s="74"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="74"/>
+      <c r="T10" s="74"/>
+      <c r="U10" s="74"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="74"/>
+      <c r="X10" s="74"/>
+      <c r="Y10" s="74"/>
+      <c r="Z10" s="74"/>
+      <c r="AA10" s="74"/>
+      <c r="AB10" s="75"/>
+      <c r="AC10" s="76" t="s">
         <v>19</v>
       </c>
       <c r="AD10" s="22" t="s">
@@ -1497,75 +1497,75 @@
       <c r="AE10" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="AF10" s="56" t="s">
+      <c r="AF10" s="81" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:39" s="10" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="57" t="s">
+      <c r="B11" s="81"/>
+      <c r="C11" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="59" t="s">
+      <c r="E11" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="60" t="s">
+      <c r="F11" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G11" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="59" t="s">
+      <c r="H11" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="59" t="s">
+      <c r="J11" s="84" t="s">
         <v>73</v>
       </c>
-      <c r="K11" s="57" t="s">
+      <c r="K11" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="L11" s="57" t="s">
+      <c r="L11" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="M11" s="62" t="s">
+      <c r="M11" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="63"/>
-      <c r="Q11" s="63"/>
-      <c r="R11" s="63"/>
-      <c r="S11" s="64"/>
-      <c r="T11" s="62" t="s">
+      <c r="N11" s="71"/>
+      <c r="O11" s="71"/>
+      <c r="P11" s="71"/>
+      <c r="Q11" s="71"/>
+      <c r="R11" s="71"/>
+      <c r="S11" s="72"/>
+      <c r="T11" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="U11" s="63"/>
-      <c r="V11" s="63"/>
-      <c r="W11" s="63"/>
-      <c r="X11" s="64"/>
-      <c r="Y11" s="62" t="s">
+      <c r="U11" s="71"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="71"/>
+      <c r="X11" s="72"/>
+      <c r="Y11" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="Z11" s="63"/>
-      <c r="AA11" s="63"/>
-      <c r="AB11" s="64"/>
-      <c r="AC11" s="67"/>
+      <c r="Z11" s="71"/>
+      <c r="AA11" s="71"/>
+      <c r="AB11" s="72"/>
+      <c r="AC11" s="77"/>
       <c r="AD11" s="25" t="s">
         <v>77</v>
       </c>
       <c r="AE11" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="AF11" s="56"/>
+      <c r="AF11" s="81"/>
     </row>
     <row r="12" spans="1:39" s="10" customFormat="1" ht="124.5" customHeight="1">
       <c r="A12" s="25" t="s">
@@ -1574,16 +1574,16 @@
       <c r="B12" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
       <c r="M12" s="24" t="s">
         <v>28</v>
       </c>
@@ -1632,14 +1632,14 @@
       <c r="AB12" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AC12" s="68"/>
+      <c r="AC12" s="78"/>
       <c r="AD12" s="24" t="s">
         <v>44</v>
       </c>
       <c r="AE12" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="AF12" s="56"/>
+      <c r="AF12" s="81"/>
     </row>
     <row r="13" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
       <c r="A13" s="11"/>
@@ -4031,43 +4031,43 @@
       <c r="D84" s="16"/>
       <c r="E84" s="16"/>
       <c r="F84" s="16"/>
-      <c r="H84" s="71" t="s">
+      <c r="H84" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="I84" s="72"/>
-      <c r="J84" s="72"/>
-      <c r="K84" s="72"/>
-      <c r="L84" s="53"/>
-      <c r="M84" s="54"/>
-      <c r="N84" s="53"/>
-      <c r="O84" s="55"/>
-      <c r="P84" s="55"/>
+      <c r="I84" s="53"/>
+      <c r="J84" s="53"/>
+      <c r="K84" s="53"/>
+      <c r="L84" s="54"/>
+      <c r="M84" s="55"/>
+      <c r="N84" s="54"/>
+      <c r="O84" s="56"/>
+      <c r="P84" s="56"/>
       <c r="Q84" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R84" s="13"/>
-      <c r="S84" s="53" t="s">
+      <c r="S84" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="T84" s="55"/>
-      <c r="U84" s="55"/>
-      <c r="V84" s="55"/>
-      <c r="W84" s="55"/>
-      <c r="X84" s="54"/>
-      <c r="Y84" s="53" t="s">
+      <c r="T84" s="56"/>
+      <c r="U84" s="56"/>
+      <c r="V84" s="56"/>
+      <c r="W84" s="56"/>
+      <c r="X84" s="55"/>
+      <c r="Y84" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="Z84" s="55"/>
-      <c r="AA84" s="54"/>
-      <c r="AB84" s="85" t="s">
+      <c r="Z84" s="56"/>
+      <c r="AA84" s="55"/>
+      <c r="AB84" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="AC84" s="85"/>
-      <c r="AD84" s="85"/>
-      <c r="AE84" s="69" t="s">
+      <c r="AC84" s="69"/>
+      <c r="AD84" s="69"/>
+      <c r="AE84" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="AF84" s="70"/>
+      <c r="AF84" s="80"/>
     </row>
     <row r="85" spans="1:32" s="18" customFormat="1" ht="17.25" customHeight="1">
       <c r="A85" s="15"/>
@@ -4077,136 +4077,202 @@
       <c r="E85" s="16"/>
       <c r="F85" s="16"/>
       <c r="G85" s="14"/>
-      <c r="H85" s="71" t="s">
+      <c r="H85" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="I85" s="72"/>
-      <c r="J85" s="72"/>
-      <c r="K85" s="72"/>
-      <c r="L85" s="53"/>
-      <c r="M85" s="54"/>
-      <c r="N85" s="53"/>
-      <c r="O85" s="55"/>
-      <c r="P85" s="55"/>
+      <c r="I85" s="53"/>
+      <c r="J85" s="53"/>
+      <c r="K85" s="53"/>
+      <c r="L85" s="54"/>
+      <c r="M85" s="55"/>
+      <c r="N85" s="54"/>
+      <c r="O85" s="56"/>
+      <c r="P85" s="56"/>
       <c r="Q85" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R85" s="13"/>
-      <c r="S85" s="73" t="s">
+      <c r="S85" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="T85" s="74"/>
-      <c r="U85" s="74"/>
-      <c r="V85" s="74"/>
-      <c r="W85" s="74"/>
-      <c r="X85" s="75"/>
-      <c r="Y85" s="79"/>
-      <c r="Z85" s="80"/>
-      <c r="AA85" s="81"/>
-      <c r="AB85" s="85"/>
-      <c r="AC85" s="85"/>
-      <c r="AD85" s="85"/>
+      <c r="T85" s="58"/>
+      <c r="U85" s="58"/>
+      <c r="V85" s="58"/>
+      <c r="W85" s="58"/>
+      <c r="X85" s="59"/>
+      <c r="Y85" s="63"/>
+      <c r="Z85" s="64"/>
+      <c r="AA85" s="65"/>
+      <c r="AB85" s="69"/>
+      <c r="AC85" s="69"/>
+      <c r="AD85" s="69"/>
       <c r="AE85" s="20"/>
       <c r="AF85" s="21"/>
     </row>
     <row r="86" spans="1:32" s="18" customFormat="1" ht="17.25" customHeight="1">
-      <c r="H86" s="71" t="s">
+      <c r="H86" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="I86" s="72"/>
-      <c r="J86" s="72"/>
-      <c r="K86" s="72"/>
-      <c r="L86" s="53"/>
-      <c r="M86" s="54"/>
-      <c r="N86" s="53"/>
-      <c r="O86" s="55"/>
-      <c r="P86" s="55"/>
+      <c r="I86" s="53"/>
+      <c r="J86" s="53"/>
+      <c r="K86" s="53"/>
+      <c r="L86" s="54"/>
+      <c r="M86" s="55"/>
+      <c r="N86" s="54"/>
+      <c r="O86" s="56"/>
+      <c r="P86" s="56"/>
       <c r="Q86" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R86" s="13"/>
-      <c r="S86" s="76"/>
-      <c r="T86" s="77"/>
-      <c r="U86" s="77"/>
-      <c r="V86" s="77"/>
-      <c r="W86" s="77"/>
-      <c r="X86" s="78"/>
-      <c r="Y86" s="82"/>
-      <c r="Z86" s="83"/>
-      <c r="AA86" s="84"/>
-      <c r="AB86" s="85"/>
-      <c r="AC86" s="85"/>
-      <c r="AD86" s="85"/>
+      <c r="S86" s="60"/>
+      <c r="T86" s="61"/>
+      <c r="U86" s="61"/>
+      <c r="V86" s="61"/>
+      <c r="W86" s="61"/>
+      <c r="X86" s="62"/>
+      <c r="Y86" s="66"/>
+      <c r="Z86" s="67"/>
+      <c r="AA86" s="68"/>
+      <c r="AB86" s="69"/>
+      <c r="AC86" s="69"/>
+      <c r="AD86" s="69"/>
     </row>
     <row r="87" spans="1:32" s="18" customFormat="1" ht="17.25" customHeight="1">
       <c r="A87" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H87" s="71" t="s">
+      <c r="H87" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="I87" s="72"/>
-      <c r="J87" s="72"/>
-      <c r="K87" s="72"/>
-      <c r="L87" s="53"/>
-      <c r="M87" s="54"/>
-      <c r="N87" s="53"/>
-      <c r="O87" s="55"/>
-      <c r="P87" s="55"/>
+      <c r="I87" s="53"/>
+      <c r="J87" s="53"/>
+      <c r="K87" s="53"/>
+      <c r="L87" s="54"/>
+      <c r="M87" s="55"/>
+      <c r="N87" s="54"/>
+      <c r="O87" s="56"/>
+      <c r="P87" s="56"/>
       <c r="Q87" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R87" s="13"/>
-      <c r="S87" s="73" t="s">
+      <c r="S87" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="T87" s="74"/>
-      <c r="U87" s="74"/>
-      <c r="V87" s="74"/>
-      <c r="W87" s="74"/>
-      <c r="X87" s="75"/>
-      <c r="Y87" s="79"/>
-      <c r="Z87" s="80"/>
-      <c r="AA87" s="81"/>
-      <c r="AB87" s="85"/>
-      <c r="AC87" s="85"/>
-      <c r="AD87" s="85"/>
+      <c r="T87" s="58"/>
+      <c r="U87" s="58"/>
+      <c r="V87" s="58"/>
+      <c r="W87" s="58"/>
+      <c r="X87" s="59"/>
+      <c r="Y87" s="63"/>
+      <c r="Z87" s="64"/>
+      <c r="AA87" s="65"/>
+      <c r="AB87" s="69"/>
+      <c r="AC87" s="69"/>
+      <c r="AD87" s="69"/>
     </row>
     <row r="88" spans="1:32" s="18" customFormat="1" ht="17.25" customHeight="1">
       <c r="A88" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H88" s="71" t="s">
+      <c r="H88" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="I88" s="72"/>
-      <c r="J88" s="72"/>
-      <c r="K88" s="72"/>
-      <c r="L88" s="53"/>
-      <c r="M88" s="54"/>
-      <c r="N88" s="53"/>
-      <c r="O88" s="55"/>
-      <c r="P88" s="55"/>
+      <c r="I88" s="53"/>
+      <c r="J88" s="53"/>
+      <c r="K88" s="53"/>
+      <c r="L88" s="54"/>
+      <c r="M88" s="55"/>
+      <c r="N88" s="54"/>
+      <c r="O88" s="56"/>
+      <c r="P88" s="56"/>
       <c r="Q88" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R88" s="13"/>
-      <c r="S88" s="76"/>
-      <c r="T88" s="77"/>
-      <c r="U88" s="77"/>
-      <c r="V88" s="77"/>
-      <c r="W88" s="77"/>
-      <c r="X88" s="78"/>
-      <c r="Y88" s="82"/>
-      <c r="Z88" s="83"/>
-      <c r="AA88" s="84"/>
-      <c r="AB88" s="85"/>
-      <c r="AC88" s="85"/>
-      <c r="AD88" s="85"/>
+      <c r="S88" s="60"/>
+      <c r="T88" s="61"/>
+      <c r="U88" s="61"/>
+      <c r="V88" s="61"/>
+      <c r="W88" s="61"/>
+      <c r="X88" s="62"/>
+      <c r="Y88" s="66"/>
+      <c r="Z88" s="67"/>
+      <c r="AA88" s="68"/>
+      <c r="AB88" s="69"/>
+      <c r="AC88" s="69"/>
+      <c r="AD88" s="69"/>
     </row>
     <row r="89" spans="1:32" s="18" customFormat="1" ht="14.25"/>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="T7:U8"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="R7:S8"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="N7:O8"/>
+    <mergeCell ref="P7:Q8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="L84:M84"/>
+    <mergeCell ref="N84:P84"/>
+    <mergeCell ref="AF10:AF12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="Y11:AB11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:S11"/>
+    <mergeCell ref="M10:AB10"/>
+    <mergeCell ref="AC10:AC12"/>
+    <mergeCell ref="AE84:AF84"/>
+    <mergeCell ref="H85:K85"/>
+    <mergeCell ref="L85:M85"/>
+    <mergeCell ref="N85:P85"/>
+    <mergeCell ref="S85:X86"/>
+    <mergeCell ref="Y85:AA86"/>
+    <mergeCell ref="AB85:AD86"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="L86:M86"/>
+    <mergeCell ref="N86:P86"/>
+    <mergeCell ref="AB84:AD84"/>
+    <mergeCell ref="Y84:AA84"/>
+    <mergeCell ref="H84:K84"/>
+    <mergeCell ref="S84:X84"/>
+    <mergeCell ref="N87:P87"/>
+    <mergeCell ref="S87:X88"/>
+    <mergeCell ref="Y87:AA88"/>
+    <mergeCell ref="AB87:AD88"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="L88:M88"/>
+    <mergeCell ref="N88:P88"/>
+    <mergeCell ref="H87:K87"/>
+    <mergeCell ref="L87:M87"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AB6:AD6"/>
@@ -4223,72 +4289,6 @@
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="D8:H8"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="L88:M88"/>
-    <mergeCell ref="N88:P88"/>
-    <mergeCell ref="H87:K87"/>
-    <mergeCell ref="L87:M87"/>
-    <mergeCell ref="S84:X84"/>
-    <mergeCell ref="N87:P87"/>
-    <mergeCell ref="S87:X88"/>
-    <mergeCell ref="Y87:AA88"/>
-    <mergeCell ref="AB87:AD88"/>
-    <mergeCell ref="M11:S11"/>
-    <mergeCell ref="M10:AB10"/>
-    <mergeCell ref="AC10:AC12"/>
-    <mergeCell ref="AE84:AF84"/>
-    <mergeCell ref="H85:K85"/>
-    <mergeCell ref="L85:M85"/>
-    <mergeCell ref="N85:P85"/>
-    <mergeCell ref="S85:X86"/>
-    <mergeCell ref="Y85:AA86"/>
-    <mergeCell ref="AB85:AD86"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="L86:M86"/>
-    <mergeCell ref="N86:P86"/>
-    <mergeCell ref="AB84:AD84"/>
-    <mergeCell ref="Y84:AA84"/>
-    <mergeCell ref="H84:K84"/>
-    <mergeCell ref="L84:M84"/>
-    <mergeCell ref="N84:P84"/>
-    <mergeCell ref="AF10:AF12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="Y11:AB11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="R7:S8"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="N7:O8"/>
-    <mergeCell ref="P7:Q8"/>
-    <mergeCell ref="T7:U8"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="AE6:AF6"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:C8 J6:K8 N6:W6 A3:AF4 AB6:AD8 A10:E12 G10:H10 J10:K10 F11:AB12 M10:AB10 Q84:AF88 A84:K88 A1:AE2 AC10:AF12" xr:uid="{01C90C96-D563-415B-B968-F3ADF92B0BE3}">
@@ -4308,7 +4308,7 @@
   </sheetPr>
   <dimension ref="A1:AM89"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -4327,10 +4327,10 @@
         <v>0</v>
       </c>
       <c r="AD1" s="3"/>
-      <c r="AE1" s="87" t="s">
+      <c r="AE1" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="AF1" s="87"/>
+      <c r="AF1" s="38"/>
       <c r="AI1" s="2"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
@@ -4341,260 +4341,260 @@
       <c r="A2" s="1"/>
       <c r="AC2" s="4"/>
       <c r="AD2" s="4"/>
-      <c r="AE2" s="86" t="s">
+      <c r="AE2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="AF2" s="86"/>
+      <c r="AF2" s="37"/>
     </row>
     <row r="3" spans="1:39" s="30" customFormat="1" ht="26.25">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="89"/>
-      <c r="T3" s="89"/>
-      <c r="U3" s="89"/>
-      <c r="V3" s="89"/>
-      <c r="W3" s="89"/>
-      <c r="X3" s="89"/>
-      <c r="Y3" s="89"/>
-      <c r="Z3" s="89"/>
-      <c r="AA3" s="89"/>
-      <c r="AB3" s="89"/>
-      <c r="AC3" s="89"/>
-      <c r="AD3" s="89"/>
-      <c r="AE3" s="89"/>
-      <c r="AF3" s="89"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="41"/>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="41"/>
+      <c r="AD3" s="41"/>
+      <c r="AE3" s="41"/>
+      <c r="AF3" s="41"/>
     </row>
     <row r="4" spans="1:39" s="29" customFormat="1" ht="19.5">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="90"/>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="90"/>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-      <c r="AB4" s="90"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="90"/>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="90"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="42"/>
+      <c r="X4" s="42"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="42"/>
+      <c r="AA4" s="42"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="42"/>
+      <c r="AD4" s="42"/>
+      <c r="AE4" s="42"/>
+      <c r="AF4" s="42"/>
     </row>
     <row r="5" spans="1:39" s="33" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="AC5" s="91"/>
-      <c r="AD5" s="91"/>
-      <c r="AE5" s="92"/>
-      <c r="AF5" s="92"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="AC5" s="44"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="45"/>
+      <c r="AF5" s="45"/>
     </row>
     <row r="6" spans="1:39" s="33" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="J6" s="47" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="J6" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="47"/>
+      <c r="K6" s="51"/>
       <c r="L6" s="27"/>
-      <c r="N6" s="42" t="s">
+      <c r="N6" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="43"/>
-      <c r="P6" s="42" t="s">
+      <c r="O6" s="91"/>
+      <c r="P6" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="42" t="s">
+      <c r="Q6" s="91"/>
+      <c r="R6" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="43"/>
-      <c r="T6" s="42" t="s">
+      <c r="S6" s="91"/>
+      <c r="T6" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="U6" s="43"/>
-      <c r="V6" s="42" t="s">
+      <c r="U6" s="91"/>
+      <c r="V6" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="W6" s="43"/>
-      <c r="AB6" s="45" t="s">
+      <c r="W6" s="91"/>
+      <c r="AB6" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="AC6" s="45"/>
-      <c r="AD6" s="88"/>
-      <c r="AE6" s="44"/>
-      <c r="AF6" s="41"/>
+      <c r="AC6" s="39"/>
+      <c r="AD6" s="40"/>
+      <c r="AE6" s="92"/>
+      <c r="AF6" s="50"/>
     </row>
     <row r="7" spans="1:39" s="33" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="J7" s="47" t="s">
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="J7" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="47"/>
+      <c r="K7" s="51"/>
       <c r="L7" s="27"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="38"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="38"/>
-      <c r="AB7" s="45" t="s">
+      <c r="N7" s="46"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="47"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="47"/>
+      <c r="AB7" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="AC7" s="45"/>
-      <c r="AD7" s="88"/>
-      <c r="AE7" s="41"/>
-      <c r="AF7" s="41"/>
+      <c r="AC7" s="39"/>
+      <c r="AD7" s="40"/>
+      <c r="AE7" s="50"/>
+      <c r="AF7" s="50"/>
     </row>
     <row r="8" spans="1:39" s="33" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="J8" s="47" t="s">
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="J8" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="47"/>
+      <c r="K8" s="51"/>
       <c r="L8" s="27"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="40"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="40"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="40"/>
-      <c r="AB8" s="45" t="s">
+      <c r="N8" s="48"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="49"/>
+      <c r="AB8" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="AC8" s="45"/>
-      <c r="AD8" s="88"/>
-      <c r="AE8" s="41"/>
-      <c r="AF8" s="41"/>
+      <c r="AC8" s="39"/>
+      <c r="AD8" s="40"/>
+      <c r="AE8" s="50"/>
+      <c r="AF8" s="50"/>
     </row>
     <row r="9" spans="1:39" s="33" customFormat="1" ht="6" customHeight="1">
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
     </row>
     <row r="10" spans="1:39" s="34" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="51" t="s">
+      <c r="B10" s="75"/>
+      <c r="C10" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
       <c r="F10" s="31"/>
-      <c r="G10" s="51" t="s">
+      <c r="G10" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="52"/>
+      <c r="H10" s="89"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="51" t="s">
+      <c r="J10" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="K10" s="52"/>
+      <c r="K10" s="89"/>
       <c r="L10" s="32"/>
-      <c r="M10" s="49" t="s">
+      <c r="M10" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="65"/>
-      <c r="O10" s="65"/>
-      <c r="P10" s="65"/>
-      <c r="Q10" s="65"/>
-      <c r="R10" s="65"/>
-      <c r="S10" s="65"/>
-      <c r="T10" s="65"/>
-      <c r="U10" s="65"/>
-      <c r="V10" s="65"/>
-      <c r="W10" s="65"/>
-      <c r="X10" s="65"/>
-      <c r="Y10" s="65"/>
-      <c r="Z10" s="65"/>
-      <c r="AA10" s="65"/>
-      <c r="AB10" s="50"/>
-      <c r="AC10" s="66" t="s">
+      <c r="N10" s="74"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="74"/>
+      <c r="T10" s="74"/>
+      <c r="U10" s="74"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="74"/>
+      <c r="X10" s="74"/>
+      <c r="Y10" s="74"/>
+      <c r="Z10" s="74"/>
+      <c r="AA10" s="74"/>
+      <c r="AB10" s="75"/>
+      <c r="AC10" s="76" t="s">
         <v>19</v>
       </c>
       <c r="AD10" s="35" t="s">
@@ -4603,75 +4603,75 @@
       <c r="AE10" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="AF10" s="56" t="s">
+      <c r="AF10" s="81" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:39" s="10" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="57" t="s">
+      <c r="B11" s="81"/>
+      <c r="C11" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="59" t="s">
+      <c r="E11" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="60" t="s">
+      <c r="F11" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G11" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="59" t="s">
+      <c r="H11" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="59" t="s">
+      <c r="J11" s="84" t="s">
         <v>73</v>
       </c>
-      <c r="K11" s="57" t="s">
+      <c r="K11" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="L11" s="57" t="s">
+      <c r="L11" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="M11" s="62" t="s">
+      <c r="M11" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="63"/>
-      <c r="Q11" s="63"/>
-      <c r="R11" s="63"/>
-      <c r="S11" s="64"/>
-      <c r="T11" s="62" t="s">
+      <c r="N11" s="71"/>
+      <c r="O11" s="71"/>
+      <c r="P11" s="71"/>
+      <c r="Q11" s="71"/>
+      <c r="R11" s="71"/>
+      <c r="S11" s="72"/>
+      <c r="T11" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="U11" s="63"/>
-      <c r="V11" s="63"/>
-      <c r="W11" s="63"/>
-      <c r="X11" s="64"/>
-      <c r="Y11" s="62" t="s">
+      <c r="U11" s="71"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="71"/>
+      <c r="X11" s="72"/>
+      <c r="Y11" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="Z11" s="63"/>
-      <c r="AA11" s="63"/>
-      <c r="AB11" s="64"/>
-      <c r="AC11" s="67"/>
+      <c r="Z11" s="71"/>
+      <c r="AA11" s="71"/>
+      <c r="AB11" s="72"/>
+      <c r="AC11" s="77"/>
       <c r="AD11" s="25" t="s">
         <v>77</v>
       </c>
       <c r="AE11" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="AF11" s="56"/>
+      <c r="AF11" s="81"/>
     </row>
     <row r="12" spans="1:39" s="10" customFormat="1" ht="124.5" customHeight="1">
       <c r="A12" s="25" t="s">
@@ -4680,16 +4680,16 @@
       <c r="B12" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
       <c r="M12" s="36" t="s">
         <v>28</v>
       </c>
@@ -4738,14 +4738,14 @@
       <c r="AB12" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="AC12" s="68"/>
+      <c r="AC12" s="78"/>
       <c r="AD12" s="36" t="s">
         <v>44</v>
       </c>
       <c r="AE12" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="AF12" s="56"/>
+      <c r="AF12" s="81"/>
     </row>
     <row r="13" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
       <c r="A13" s="11"/>
@@ -7137,43 +7137,43 @@
       <c r="D84" s="16"/>
       <c r="E84" s="16"/>
       <c r="F84" s="16"/>
-      <c r="H84" s="71" t="s">
+      <c r="H84" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="I84" s="72"/>
-      <c r="J84" s="72"/>
-      <c r="K84" s="72"/>
-      <c r="L84" s="53"/>
-      <c r="M84" s="54"/>
-      <c r="N84" s="53"/>
-      <c r="O84" s="55"/>
-      <c r="P84" s="55"/>
+      <c r="I84" s="53"/>
+      <c r="J84" s="53"/>
+      <c r="K84" s="53"/>
+      <c r="L84" s="54"/>
+      <c r="M84" s="55"/>
+      <c r="N84" s="54"/>
+      <c r="O84" s="56"/>
+      <c r="P84" s="56"/>
       <c r="Q84" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R84" s="13"/>
-      <c r="S84" s="53" t="s">
+      <c r="S84" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="T84" s="55"/>
-      <c r="U84" s="55"/>
-      <c r="V84" s="55"/>
-      <c r="W84" s="55"/>
-      <c r="X84" s="54"/>
-      <c r="Y84" s="53" t="s">
+      <c r="T84" s="56"/>
+      <c r="U84" s="56"/>
+      <c r="V84" s="56"/>
+      <c r="W84" s="56"/>
+      <c r="X84" s="55"/>
+      <c r="Y84" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="Z84" s="55"/>
-      <c r="AA84" s="54"/>
-      <c r="AB84" s="85" t="s">
+      <c r="Z84" s="56"/>
+      <c r="AA84" s="55"/>
+      <c r="AB84" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="AC84" s="85"/>
-      <c r="AD84" s="85"/>
-      <c r="AE84" s="69" t="s">
+      <c r="AC84" s="69"/>
+      <c r="AD84" s="69"/>
+      <c r="AE84" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="AF84" s="70"/>
+      <c r="AF84" s="80"/>
     </row>
     <row r="85" spans="1:32" s="18" customFormat="1" ht="17.25" customHeight="1">
       <c r="A85" s="15"/>
@@ -7183,194 +7183,144 @@
       <c r="E85" s="16"/>
       <c r="F85" s="16"/>
       <c r="G85" s="14"/>
-      <c r="H85" s="71" t="s">
+      <c r="H85" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="I85" s="72"/>
-      <c r="J85" s="72"/>
-      <c r="K85" s="72"/>
-      <c r="L85" s="53"/>
-      <c r="M85" s="54"/>
-      <c r="N85" s="53"/>
-      <c r="O85" s="55"/>
-      <c r="P85" s="55"/>
+      <c r="I85" s="53"/>
+      <c r="J85" s="53"/>
+      <c r="K85" s="53"/>
+      <c r="L85" s="54"/>
+      <c r="M85" s="55"/>
+      <c r="N85" s="54"/>
+      <c r="O85" s="56"/>
+      <c r="P85" s="56"/>
       <c r="Q85" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R85" s="13"/>
-      <c r="S85" s="73" t="s">
+      <c r="S85" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="T85" s="74"/>
-      <c r="U85" s="74"/>
-      <c r="V85" s="74"/>
-      <c r="W85" s="74"/>
-      <c r="X85" s="75"/>
-      <c r="Y85" s="79"/>
-      <c r="Z85" s="80"/>
-      <c r="AA85" s="81"/>
-      <c r="AB85" s="85"/>
-      <c r="AC85" s="85"/>
-      <c r="AD85" s="85"/>
+      <c r="T85" s="58"/>
+      <c r="U85" s="58"/>
+      <c r="V85" s="58"/>
+      <c r="W85" s="58"/>
+      <c r="X85" s="59"/>
+      <c r="Y85" s="63"/>
+      <c r="Z85" s="64"/>
+      <c r="AA85" s="65"/>
+      <c r="AB85" s="69"/>
+      <c r="AC85" s="69"/>
+      <c r="AD85" s="69"/>
       <c r="AE85" s="20"/>
       <c r="AF85" s="21"/>
     </row>
     <row r="86" spans="1:32" s="18" customFormat="1" ht="17.25" customHeight="1">
-      <c r="H86" s="71" t="s">
+      <c r="H86" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="I86" s="72"/>
-      <c r="J86" s="72"/>
-      <c r="K86" s="72"/>
-      <c r="L86" s="53"/>
-      <c r="M86" s="54"/>
-      <c r="N86" s="53"/>
-      <c r="O86" s="55"/>
-      <c r="P86" s="55"/>
+      <c r="I86" s="53"/>
+      <c r="J86" s="53"/>
+      <c r="K86" s="53"/>
+      <c r="L86" s="54"/>
+      <c r="M86" s="55"/>
+      <c r="N86" s="54"/>
+      <c r="O86" s="56"/>
+      <c r="P86" s="56"/>
       <c r="Q86" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R86" s="13"/>
-      <c r="S86" s="76"/>
-      <c r="T86" s="77"/>
-      <c r="U86" s="77"/>
-      <c r="V86" s="77"/>
-      <c r="W86" s="77"/>
-      <c r="X86" s="78"/>
-      <c r="Y86" s="82"/>
-      <c r="Z86" s="83"/>
-      <c r="AA86" s="84"/>
-      <c r="AB86" s="85"/>
-      <c r="AC86" s="85"/>
-      <c r="AD86" s="85"/>
+      <c r="S86" s="60"/>
+      <c r="T86" s="61"/>
+      <c r="U86" s="61"/>
+      <c r="V86" s="61"/>
+      <c r="W86" s="61"/>
+      <c r="X86" s="62"/>
+      <c r="Y86" s="66"/>
+      <c r="Z86" s="67"/>
+      <c r="AA86" s="68"/>
+      <c r="AB86" s="69"/>
+      <c r="AC86" s="69"/>
+      <c r="AD86" s="69"/>
     </row>
     <row r="87" spans="1:32" s="18" customFormat="1" ht="17.25" customHeight="1">
       <c r="A87" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H87" s="71" t="s">
+      <c r="H87" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="I87" s="72"/>
-      <c r="J87" s="72"/>
-      <c r="K87" s="72"/>
-      <c r="L87" s="53"/>
-      <c r="M87" s="54"/>
-      <c r="N87" s="53"/>
-      <c r="O87" s="55"/>
-      <c r="P87" s="55"/>
+      <c r="I87" s="53"/>
+      <c r="J87" s="53"/>
+      <c r="K87" s="53"/>
+      <c r="L87" s="54"/>
+      <c r="M87" s="55"/>
+      <c r="N87" s="54"/>
+      <c r="O87" s="56"/>
+      <c r="P87" s="56"/>
       <c r="Q87" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R87" s="13"/>
-      <c r="S87" s="73" t="s">
+      <c r="S87" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="T87" s="74"/>
-      <c r="U87" s="74"/>
-      <c r="V87" s="74"/>
-      <c r="W87" s="74"/>
-      <c r="X87" s="75"/>
-      <c r="Y87" s="79"/>
-      <c r="Z87" s="80"/>
-      <c r="AA87" s="81"/>
-      <c r="AB87" s="85"/>
-      <c r="AC87" s="85"/>
-      <c r="AD87" s="85"/>
+      <c r="T87" s="58"/>
+      <c r="U87" s="58"/>
+      <c r="V87" s="58"/>
+      <c r="W87" s="58"/>
+      <c r="X87" s="59"/>
+      <c r="Y87" s="63"/>
+      <c r="Z87" s="64"/>
+      <c r="AA87" s="65"/>
+      <c r="AB87" s="69"/>
+      <c r="AC87" s="69"/>
+      <c r="AD87" s="69"/>
     </row>
     <row r="88" spans="1:32" s="18" customFormat="1" ht="17.25" customHeight="1">
       <c r="A88" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H88" s="71" t="s">
+      <c r="H88" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="I88" s="72"/>
-      <c r="J88" s="72"/>
-      <c r="K88" s="72"/>
-      <c r="L88" s="53"/>
-      <c r="M88" s="54"/>
-      <c r="N88" s="53"/>
-      <c r="O88" s="55"/>
-      <c r="P88" s="55"/>
+      <c r="I88" s="53"/>
+      <c r="J88" s="53"/>
+      <c r="K88" s="53"/>
+      <c r="L88" s="54"/>
+      <c r="M88" s="55"/>
+      <c r="N88" s="54"/>
+      <c r="O88" s="56"/>
+      <c r="P88" s="56"/>
       <c r="Q88" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R88" s="13"/>
-      <c r="S88" s="76"/>
-      <c r="T88" s="77"/>
-      <c r="U88" s="77"/>
-      <c r="V88" s="77"/>
-      <c r="W88" s="77"/>
-      <c r="X88" s="78"/>
-      <c r="Y88" s="82"/>
-      <c r="Z88" s="83"/>
-      <c r="AA88" s="84"/>
-      <c r="AB88" s="85"/>
-      <c r="AC88" s="85"/>
-      <c r="AD88" s="85"/>
+      <c r="S88" s="60"/>
+      <c r="T88" s="61"/>
+      <c r="U88" s="61"/>
+      <c r="V88" s="61"/>
+      <c r="W88" s="61"/>
+      <c r="X88" s="62"/>
+      <c r="Y88" s="66"/>
+      <c r="Z88" s="67"/>
+      <c r="AA88" s="68"/>
+      <c r="AB88" s="69"/>
+      <c r="AC88" s="69"/>
+      <c r="AD88" s="69"/>
     </row>
     <row r="89" spans="1:32" s="18" customFormat="1" ht="14.25"/>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="H87:K87"/>
-    <mergeCell ref="L87:M87"/>
-    <mergeCell ref="N87:P87"/>
-    <mergeCell ref="S87:X88"/>
-    <mergeCell ref="Y87:AA88"/>
-    <mergeCell ref="AB87:AD88"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="L88:M88"/>
-    <mergeCell ref="N88:P88"/>
-    <mergeCell ref="AE84:AF84"/>
-    <mergeCell ref="H85:K85"/>
-    <mergeCell ref="L85:M85"/>
-    <mergeCell ref="N85:P85"/>
-    <mergeCell ref="S85:X86"/>
-    <mergeCell ref="Y85:AA86"/>
-    <mergeCell ref="AB85:AD86"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="L86:M86"/>
-    <mergeCell ref="N86:P86"/>
-    <mergeCell ref="Y11:AB11"/>
-    <mergeCell ref="H84:K84"/>
-    <mergeCell ref="L84:M84"/>
-    <mergeCell ref="N84:P84"/>
-    <mergeCell ref="S84:X84"/>
-    <mergeCell ref="Y84:AA84"/>
-    <mergeCell ref="AB84:AD84"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:S11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="M10:AB10"/>
-    <mergeCell ref="AC10:AC12"/>
-    <mergeCell ref="AF10:AF12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="T7:U8"/>
-    <mergeCell ref="V7:W8"/>
-    <mergeCell ref="AB7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="AB8:AD8"/>
-    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="A3:AF3"/>
+    <mergeCell ref="A4:AF4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="V6:W6"/>
     <mergeCell ref="AB6:AD6"/>
@@ -7387,14 +7337,64 @@
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:Q6"/>
     <mergeCell ref="R6:S6"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="A3:AF3"/>
-    <mergeCell ref="A4:AF4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="T7:U8"/>
+    <mergeCell ref="V7:W8"/>
+    <mergeCell ref="AB7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="AB8:AD8"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="M10:AB10"/>
+    <mergeCell ref="AC10:AC12"/>
+    <mergeCell ref="AF10:AF12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="Y11:AB11"/>
+    <mergeCell ref="H84:K84"/>
+    <mergeCell ref="L84:M84"/>
+    <mergeCell ref="N84:P84"/>
+    <mergeCell ref="S84:X84"/>
+    <mergeCell ref="Y84:AA84"/>
+    <mergeCell ref="AB84:AD84"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:S11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="AB87:AD88"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="L88:M88"/>
+    <mergeCell ref="N88:P88"/>
+    <mergeCell ref="AE84:AF84"/>
+    <mergeCell ref="H85:K85"/>
+    <mergeCell ref="L85:M85"/>
+    <mergeCell ref="N85:P85"/>
+    <mergeCell ref="S85:X86"/>
+    <mergeCell ref="Y85:AA86"/>
+    <mergeCell ref="AB85:AD86"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="L86:M86"/>
+    <mergeCell ref="N86:P86"/>
+    <mergeCell ref="H87:K87"/>
+    <mergeCell ref="L87:M87"/>
+    <mergeCell ref="N87:P87"/>
+    <mergeCell ref="S87:X88"/>
+    <mergeCell ref="Y87:AA88"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:C8 J6:K8 N6:W6 A3:AF4 AB6:AD8 A10:E12 G10:H10 J10:K10 F11:AB12 M10:AB10 Q84:AF88 A84:K88 A1:AE2 AC10:AF12" xr:uid="{05864283-16BB-43BA-8EE6-A8A4584567D6}">
@@ -7414,7 +7414,7 @@
   </sheetPr>
   <dimension ref="A1:AM89"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -7433,10 +7433,10 @@
         <v>0</v>
       </c>
       <c r="AD1" s="3"/>
-      <c r="AE1" s="87" t="s">
+      <c r="AE1" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="AF1" s="87"/>
+      <c r="AF1" s="38"/>
       <c r="AI1" s="2"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
@@ -7447,260 +7447,260 @@
       <c r="A2" s="1"/>
       <c r="AC2" s="4"/>
       <c r="AD2" s="4"/>
-      <c r="AE2" s="86" t="s">
+      <c r="AE2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="AF2" s="86"/>
+      <c r="AF2" s="37"/>
     </row>
     <row r="3" spans="1:39" s="30" customFormat="1" ht="26.25">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="89"/>
-      <c r="T3" s="89"/>
-      <c r="U3" s="89"/>
-      <c r="V3" s="89"/>
-      <c r="W3" s="89"/>
-      <c r="X3" s="89"/>
-      <c r="Y3" s="89"/>
-      <c r="Z3" s="89"/>
-      <c r="AA3" s="89"/>
-      <c r="AB3" s="89"/>
-      <c r="AC3" s="89"/>
-      <c r="AD3" s="89"/>
-      <c r="AE3" s="89"/>
-      <c r="AF3" s="89"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="41"/>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="41"/>
+      <c r="AD3" s="41"/>
+      <c r="AE3" s="41"/>
+      <c r="AF3" s="41"/>
     </row>
     <row r="4" spans="1:39" s="29" customFormat="1" ht="19.5">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="90"/>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="90"/>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-      <c r="AB4" s="90"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="90"/>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="90"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="42"/>
+      <c r="X4" s="42"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="42"/>
+      <c r="AA4" s="42"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="42"/>
+      <c r="AD4" s="42"/>
+      <c r="AE4" s="42"/>
+      <c r="AF4" s="42"/>
     </row>
     <row r="5" spans="1:39" s="33" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="AC5" s="91"/>
-      <c r="AD5" s="91"/>
-      <c r="AE5" s="92"/>
-      <c r="AF5" s="92"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="AC5" s="44"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="45"/>
+      <c r="AF5" s="45"/>
     </row>
     <row r="6" spans="1:39" s="33" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="J6" s="47" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="J6" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="47"/>
+      <c r="K6" s="51"/>
       <c r="L6" s="27"/>
-      <c r="N6" s="42" t="s">
+      <c r="N6" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="43"/>
-      <c r="P6" s="42" t="s">
+      <c r="O6" s="91"/>
+      <c r="P6" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="42" t="s">
+      <c r="Q6" s="91"/>
+      <c r="R6" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="43"/>
-      <c r="T6" s="42" t="s">
+      <c r="S6" s="91"/>
+      <c r="T6" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="U6" s="43"/>
-      <c r="V6" s="42" t="s">
+      <c r="U6" s="91"/>
+      <c r="V6" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="W6" s="43"/>
-      <c r="AB6" s="45" t="s">
+      <c r="W6" s="91"/>
+      <c r="AB6" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="AC6" s="45"/>
-      <c r="AD6" s="88"/>
-      <c r="AE6" s="44"/>
-      <c r="AF6" s="41"/>
+      <c r="AC6" s="39"/>
+      <c r="AD6" s="40"/>
+      <c r="AE6" s="92"/>
+      <c r="AF6" s="50"/>
     </row>
     <row r="7" spans="1:39" s="33" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="J7" s="47" t="s">
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="J7" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="47"/>
+      <c r="K7" s="51"/>
       <c r="L7" s="27"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="38"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="38"/>
-      <c r="AB7" s="45" t="s">
+      <c r="N7" s="46"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="47"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="47"/>
+      <c r="AB7" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="AC7" s="45"/>
-      <c r="AD7" s="88"/>
-      <c r="AE7" s="41"/>
-      <c r="AF7" s="41"/>
+      <c r="AC7" s="39"/>
+      <c r="AD7" s="40"/>
+      <c r="AE7" s="50"/>
+      <c r="AF7" s="50"/>
     </row>
     <row r="8" spans="1:39" s="33" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="J8" s="47" t="s">
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="J8" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="47"/>
+      <c r="K8" s="51"/>
       <c r="L8" s="27"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="40"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="40"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="40"/>
-      <c r="AB8" s="45" t="s">
+      <c r="N8" s="48"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="49"/>
+      <c r="AB8" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="AC8" s="45"/>
-      <c r="AD8" s="88"/>
-      <c r="AE8" s="41"/>
-      <c r="AF8" s="41"/>
+      <c r="AC8" s="39"/>
+      <c r="AD8" s="40"/>
+      <c r="AE8" s="50"/>
+      <c r="AF8" s="50"/>
     </row>
     <row r="9" spans="1:39" s="33" customFormat="1" ht="6" customHeight="1">
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
     </row>
     <row r="10" spans="1:39" s="34" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="51" t="s">
+      <c r="B10" s="75"/>
+      <c r="C10" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
       <c r="F10" s="31"/>
-      <c r="G10" s="51" t="s">
+      <c r="G10" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="52"/>
+      <c r="H10" s="89"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="51" t="s">
+      <c r="J10" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="K10" s="52"/>
+      <c r="K10" s="89"/>
       <c r="L10" s="32"/>
-      <c r="M10" s="49" t="s">
+      <c r="M10" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="65"/>
-      <c r="O10" s="65"/>
-      <c r="P10" s="65"/>
-      <c r="Q10" s="65"/>
-      <c r="R10" s="65"/>
-      <c r="S10" s="65"/>
-      <c r="T10" s="65"/>
-      <c r="U10" s="65"/>
-      <c r="V10" s="65"/>
-      <c r="W10" s="65"/>
-      <c r="X10" s="65"/>
-      <c r="Y10" s="65"/>
-      <c r="Z10" s="65"/>
-      <c r="AA10" s="65"/>
-      <c r="AB10" s="50"/>
-      <c r="AC10" s="66" t="s">
+      <c r="N10" s="74"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="74"/>
+      <c r="T10" s="74"/>
+      <c r="U10" s="74"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="74"/>
+      <c r="X10" s="74"/>
+      <c r="Y10" s="74"/>
+      <c r="Z10" s="74"/>
+      <c r="AA10" s="74"/>
+      <c r="AB10" s="75"/>
+      <c r="AC10" s="76" t="s">
         <v>19</v>
       </c>
       <c r="AD10" s="35" t="s">
@@ -7709,75 +7709,75 @@
       <c r="AE10" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="AF10" s="56" t="s">
+      <c r="AF10" s="81" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:39" s="10" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="57" t="s">
+      <c r="B11" s="81"/>
+      <c r="C11" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="59" t="s">
+      <c r="E11" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="60" t="s">
+      <c r="F11" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G11" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="59" t="s">
+      <c r="H11" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="59" t="s">
+      <c r="J11" s="84" t="s">
         <v>73</v>
       </c>
-      <c r="K11" s="57" t="s">
+      <c r="K11" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="L11" s="57" t="s">
+      <c r="L11" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="M11" s="62" t="s">
+      <c r="M11" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="63"/>
-      <c r="Q11" s="63"/>
-      <c r="R11" s="63"/>
-      <c r="S11" s="64"/>
-      <c r="T11" s="62" t="s">
+      <c r="N11" s="71"/>
+      <c r="O11" s="71"/>
+      <c r="P11" s="71"/>
+      <c r="Q11" s="71"/>
+      <c r="R11" s="71"/>
+      <c r="S11" s="72"/>
+      <c r="T11" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="U11" s="63"/>
-      <c r="V11" s="63"/>
-      <c r="W11" s="63"/>
-      <c r="X11" s="64"/>
-      <c r="Y11" s="62" t="s">
+      <c r="U11" s="71"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="71"/>
+      <c r="X11" s="72"/>
+      <c r="Y11" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="Z11" s="63"/>
-      <c r="AA11" s="63"/>
-      <c r="AB11" s="64"/>
-      <c r="AC11" s="67"/>
+      <c r="Z11" s="71"/>
+      <c r="AA11" s="71"/>
+      <c r="AB11" s="72"/>
+      <c r="AC11" s="77"/>
       <c r="AD11" s="25" t="s">
         <v>77</v>
       </c>
       <c r="AE11" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="AF11" s="56"/>
+      <c r="AF11" s="81"/>
     </row>
     <row r="12" spans="1:39" s="10" customFormat="1" ht="124.5" customHeight="1">
       <c r="A12" s="25" t="s">
@@ -7786,16 +7786,16 @@
       <c r="B12" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
       <c r="M12" s="36" t="s">
         <v>28</v>
       </c>
@@ -7844,14 +7844,14 @@
       <c r="AB12" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="AC12" s="68"/>
+      <c r="AC12" s="78"/>
       <c r="AD12" s="36" t="s">
         <v>44</v>
       </c>
       <c r="AE12" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="AF12" s="56"/>
+      <c r="AF12" s="81"/>
     </row>
     <row r="13" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
       <c r="A13" s="11"/>
@@ -10243,43 +10243,43 @@
       <c r="D84" s="16"/>
       <c r="E84" s="16"/>
       <c r="F84" s="16"/>
-      <c r="H84" s="71" t="s">
+      <c r="H84" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="I84" s="72"/>
-      <c r="J84" s="72"/>
-      <c r="K84" s="72"/>
-      <c r="L84" s="53"/>
-      <c r="M84" s="54"/>
-      <c r="N84" s="53"/>
-      <c r="O84" s="55"/>
-      <c r="P84" s="55"/>
+      <c r="I84" s="53"/>
+      <c r="J84" s="53"/>
+      <c r="K84" s="53"/>
+      <c r="L84" s="54"/>
+      <c r="M84" s="55"/>
+      <c r="N84" s="54"/>
+      <c r="O84" s="56"/>
+      <c r="P84" s="56"/>
       <c r="Q84" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R84" s="13"/>
-      <c r="S84" s="53" t="s">
+      <c r="S84" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="T84" s="55"/>
-      <c r="U84" s="55"/>
-      <c r="V84" s="55"/>
-      <c r="W84" s="55"/>
-      <c r="X84" s="54"/>
-      <c r="Y84" s="53" t="s">
+      <c r="T84" s="56"/>
+      <c r="U84" s="56"/>
+      <c r="V84" s="56"/>
+      <c r="W84" s="56"/>
+      <c r="X84" s="55"/>
+      <c r="Y84" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="Z84" s="55"/>
-      <c r="AA84" s="54"/>
-      <c r="AB84" s="85" t="s">
+      <c r="Z84" s="56"/>
+      <c r="AA84" s="55"/>
+      <c r="AB84" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="AC84" s="85"/>
-      <c r="AD84" s="85"/>
-      <c r="AE84" s="69" t="s">
+      <c r="AC84" s="69"/>
+      <c r="AD84" s="69"/>
+      <c r="AE84" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="AF84" s="70"/>
+      <c r="AF84" s="80"/>
     </row>
     <row r="85" spans="1:32" s="18" customFormat="1" ht="17.25" customHeight="1">
       <c r="A85" s="15"/>
@@ -10289,194 +10289,144 @@
       <c r="E85" s="16"/>
       <c r="F85" s="16"/>
       <c r="G85" s="14"/>
-      <c r="H85" s="71" t="s">
+      <c r="H85" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="I85" s="72"/>
-      <c r="J85" s="72"/>
-      <c r="K85" s="72"/>
-      <c r="L85" s="53"/>
-      <c r="M85" s="54"/>
-      <c r="N85" s="53"/>
-      <c r="O85" s="55"/>
-      <c r="P85" s="55"/>
+      <c r="I85" s="53"/>
+      <c r="J85" s="53"/>
+      <c r="K85" s="53"/>
+      <c r="L85" s="54"/>
+      <c r="M85" s="55"/>
+      <c r="N85" s="54"/>
+      <c r="O85" s="56"/>
+      <c r="P85" s="56"/>
       <c r="Q85" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R85" s="13"/>
-      <c r="S85" s="73" t="s">
+      <c r="S85" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="T85" s="74"/>
-      <c r="U85" s="74"/>
-      <c r="V85" s="74"/>
-      <c r="W85" s="74"/>
-      <c r="X85" s="75"/>
-      <c r="Y85" s="79"/>
-      <c r="Z85" s="80"/>
-      <c r="AA85" s="81"/>
-      <c r="AB85" s="85"/>
-      <c r="AC85" s="85"/>
-      <c r="AD85" s="85"/>
+      <c r="T85" s="58"/>
+      <c r="U85" s="58"/>
+      <c r="V85" s="58"/>
+      <c r="W85" s="58"/>
+      <c r="X85" s="59"/>
+      <c r="Y85" s="63"/>
+      <c r="Z85" s="64"/>
+      <c r="AA85" s="65"/>
+      <c r="AB85" s="69"/>
+      <c r="AC85" s="69"/>
+      <c r="AD85" s="69"/>
       <c r="AE85" s="20"/>
       <c r="AF85" s="21"/>
     </row>
     <row r="86" spans="1:32" s="18" customFormat="1" ht="17.25" customHeight="1">
-      <c r="H86" s="71" t="s">
+      <c r="H86" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="I86" s="72"/>
-      <c r="J86" s="72"/>
-      <c r="K86" s="72"/>
-      <c r="L86" s="53"/>
-      <c r="M86" s="54"/>
-      <c r="N86" s="53"/>
-      <c r="O86" s="55"/>
-      <c r="P86" s="55"/>
+      <c r="I86" s="53"/>
+      <c r="J86" s="53"/>
+      <c r="K86" s="53"/>
+      <c r="L86" s="54"/>
+      <c r="M86" s="55"/>
+      <c r="N86" s="54"/>
+      <c r="O86" s="56"/>
+      <c r="P86" s="56"/>
       <c r="Q86" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R86" s="13"/>
-      <c r="S86" s="76"/>
-      <c r="T86" s="77"/>
-      <c r="U86" s="77"/>
-      <c r="V86" s="77"/>
-      <c r="W86" s="77"/>
-      <c r="X86" s="78"/>
-      <c r="Y86" s="82"/>
-      <c r="Z86" s="83"/>
-      <c r="AA86" s="84"/>
-      <c r="AB86" s="85"/>
-      <c r="AC86" s="85"/>
-      <c r="AD86" s="85"/>
+      <c r="S86" s="60"/>
+      <c r="T86" s="61"/>
+      <c r="U86" s="61"/>
+      <c r="V86" s="61"/>
+      <c r="W86" s="61"/>
+      <c r="X86" s="62"/>
+      <c r="Y86" s="66"/>
+      <c r="Z86" s="67"/>
+      <c r="AA86" s="68"/>
+      <c r="AB86" s="69"/>
+      <c r="AC86" s="69"/>
+      <c r="AD86" s="69"/>
     </row>
     <row r="87" spans="1:32" s="18" customFormat="1" ht="17.25" customHeight="1">
       <c r="A87" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H87" s="71" t="s">
+      <c r="H87" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="I87" s="72"/>
-      <c r="J87" s="72"/>
-      <c r="K87" s="72"/>
-      <c r="L87" s="53"/>
-      <c r="M87" s="54"/>
-      <c r="N87" s="53"/>
-      <c r="O87" s="55"/>
-      <c r="P87" s="55"/>
+      <c r="I87" s="53"/>
+      <c r="J87" s="53"/>
+      <c r="K87" s="53"/>
+      <c r="L87" s="54"/>
+      <c r="M87" s="55"/>
+      <c r="N87" s="54"/>
+      <c r="O87" s="56"/>
+      <c r="P87" s="56"/>
       <c r="Q87" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R87" s="13"/>
-      <c r="S87" s="73" t="s">
+      <c r="S87" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="T87" s="74"/>
-      <c r="U87" s="74"/>
-      <c r="V87" s="74"/>
-      <c r="W87" s="74"/>
-      <c r="X87" s="75"/>
-      <c r="Y87" s="79"/>
-      <c r="Z87" s="80"/>
-      <c r="AA87" s="81"/>
-      <c r="AB87" s="85"/>
-      <c r="AC87" s="85"/>
-      <c r="AD87" s="85"/>
+      <c r="T87" s="58"/>
+      <c r="U87" s="58"/>
+      <c r="V87" s="58"/>
+      <c r="W87" s="58"/>
+      <c r="X87" s="59"/>
+      <c r="Y87" s="63"/>
+      <c r="Z87" s="64"/>
+      <c r="AA87" s="65"/>
+      <c r="AB87" s="69"/>
+      <c r="AC87" s="69"/>
+      <c r="AD87" s="69"/>
     </row>
     <row r="88" spans="1:32" s="18" customFormat="1" ht="17.25" customHeight="1">
       <c r="A88" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H88" s="71" t="s">
+      <c r="H88" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="I88" s="72"/>
-      <c r="J88" s="72"/>
-      <c r="K88" s="72"/>
-      <c r="L88" s="53"/>
-      <c r="M88" s="54"/>
-      <c r="N88" s="53"/>
-      <c r="O88" s="55"/>
-      <c r="P88" s="55"/>
+      <c r="I88" s="53"/>
+      <c r="J88" s="53"/>
+      <c r="K88" s="53"/>
+      <c r="L88" s="54"/>
+      <c r="M88" s="55"/>
+      <c r="N88" s="54"/>
+      <c r="O88" s="56"/>
+      <c r="P88" s="56"/>
       <c r="Q88" s="17" t="s">
         <v>47</v>
       </c>
       <c r="R88" s="13"/>
-      <c r="S88" s="76"/>
-      <c r="T88" s="77"/>
-      <c r="U88" s="77"/>
-      <c r="V88" s="77"/>
-      <c r="W88" s="77"/>
-      <c r="X88" s="78"/>
-      <c r="Y88" s="82"/>
-      <c r="Z88" s="83"/>
-      <c r="AA88" s="84"/>
-      <c r="AB88" s="85"/>
-      <c r="AC88" s="85"/>
-      <c r="AD88" s="85"/>
+      <c r="S88" s="60"/>
+      <c r="T88" s="61"/>
+      <c r="U88" s="61"/>
+      <c r="V88" s="61"/>
+      <c r="W88" s="61"/>
+      <c r="X88" s="62"/>
+      <c r="Y88" s="66"/>
+      <c r="Z88" s="67"/>
+      <c r="AA88" s="68"/>
+      <c r="AB88" s="69"/>
+      <c r="AC88" s="69"/>
+      <c r="AD88" s="69"/>
     </row>
     <row r="89" spans="1:32" s="18" customFormat="1" ht="14.25"/>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="H87:K87"/>
-    <mergeCell ref="L87:M87"/>
-    <mergeCell ref="N87:P87"/>
-    <mergeCell ref="S87:X88"/>
-    <mergeCell ref="Y87:AA88"/>
-    <mergeCell ref="AB87:AD88"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="L88:M88"/>
-    <mergeCell ref="N88:P88"/>
-    <mergeCell ref="AE84:AF84"/>
-    <mergeCell ref="H85:K85"/>
-    <mergeCell ref="L85:M85"/>
-    <mergeCell ref="N85:P85"/>
-    <mergeCell ref="S85:X86"/>
-    <mergeCell ref="Y85:AA86"/>
-    <mergeCell ref="AB85:AD86"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="L86:M86"/>
-    <mergeCell ref="N86:P86"/>
-    <mergeCell ref="Y11:AB11"/>
-    <mergeCell ref="H84:K84"/>
-    <mergeCell ref="L84:M84"/>
-    <mergeCell ref="N84:P84"/>
-    <mergeCell ref="S84:X84"/>
-    <mergeCell ref="Y84:AA84"/>
-    <mergeCell ref="AB84:AD84"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:S11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="M10:AB10"/>
-    <mergeCell ref="AC10:AC12"/>
-    <mergeCell ref="AF10:AF12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="T7:U8"/>
-    <mergeCell ref="V7:W8"/>
-    <mergeCell ref="AB7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="AB8:AD8"/>
-    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="A3:AF3"/>
+    <mergeCell ref="A4:AF4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="V6:W6"/>
     <mergeCell ref="AB6:AD6"/>
@@ -10493,14 +10443,64 @@
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:Q6"/>
     <mergeCell ref="R6:S6"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="A3:AF3"/>
-    <mergeCell ref="A4:AF4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="T7:U8"/>
+    <mergeCell ref="V7:W8"/>
+    <mergeCell ref="AB7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="AB8:AD8"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="M10:AB10"/>
+    <mergeCell ref="AC10:AC12"/>
+    <mergeCell ref="AF10:AF12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="Y11:AB11"/>
+    <mergeCell ref="H84:K84"/>
+    <mergeCell ref="L84:M84"/>
+    <mergeCell ref="N84:P84"/>
+    <mergeCell ref="S84:X84"/>
+    <mergeCell ref="Y84:AA84"/>
+    <mergeCell ref="AB84:AD84"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:S11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="AB87:AD88"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="L88:M88"/>
+    <mergeCell ref="N88:P88"/>
+    <mergeCell ref="AE84:AF84"/>
+    <mergeCell ref="H85:K85"/>
+    <mergeCell ref="L85:M85"/>
+    <mergeCell ref="N85:P85"/>
+    <mergeCell ref="S85:X86"/>
+    <mergeCell ref="Y85:AA86"/>
+    <mergeCell ref="AB85:AD86"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="L86:M86"/>
+    <mergeCell ref="N86:P86"/>
+    <mergeCell ref="H87:K87"/>
+    <mergeCell ref="L87:M87"/>
+    <mergeCell ref="N87:P87"/>
+    <mergeCell ref="S87:X88"/>
+    <mergeCell ref="Y87:AA88"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:C8 J6:K8 N6:W6 A3:AF4 AB6:AD8 A10:E12 G10:H10 J10:K10 F11:AB12 M10:AB10 Q84:AF88 A84:K88 A1:AE2 AC10:AF12" xr:uid="{EC8ADC4C-F934-4FB8-A345-C72BE5D67CAF}">

</xml_diff>